<commit_message>
Ajuste na pontuação das tabelas
</commit_message>
<xml_diff>
--- a/brasil-clubes-rank-2024/tabelas/Campeonato Brasileiro Rank.xlsx
+++ b/brasil-clubes-rank-2024/tabelas/Campeonato Brasileiro Rank.xlsx
@@ -567,7 +567,7 @@
         <v>61</v>
       </c>
       <c r="Q2" t="n">
-        <v>48874</v>
+        <v>2036.42</v>
       </c>
     </row>
     <row r="3">
@@ -622,7 +622,7 @@
         <v>63</v>
       </c>
       <c r="Q3" t="n">
-        <v>40552</v>
+        <v>1689.67</v>
       </c>
     </row>
     <row r="4">
@@ -677,7 +677,7 @@
         <v>56</v>
       </c>
       <c r="Q4" t="n">
-        <v>35640</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="5">
@@ -732,7 +732,7 @@
         <v>59</v>
       </c>
       <c r="Q5" t="n">
-        <v>35208</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="6">
@@ -787,7 +787,7 @@
         <v>57</v>
       </c>
       <c r="Q6" t="n">
-        <v>35016</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="7">
@@ -842,7 +842,7 @@
         <v>61</v>
       </c>
       <c r="Q7" t="n">
-        <v>31462</v>
+        <v>1310.92</v>
       </c>
     </row>
     <row r="8">
@@ -897,7 +897,7 @@
         <v>62</v>
       </c>
       <c r="Q8" t="n">
-        <v>31294</v>
+        <v>1303.92</v>
       </c>
     </row>
     <row r="9">
@@ -952,7 +952,7 @@
         <v>58</v>
       </c>
       <c r="Q9" t="n">
-        <v>30220</v>
+        <v>1259.17</v>
       </c>
     </row>
     <row r="10">
@@ -1007,7 +1007,7 @@
         <v>64</v>
       </c>
       <c r="Q10" t="n">
-        <v>29948</v>
+        <v>1247.83</v>
       </c>
     </row>
     <row r="11">
@@ -1062,7 +1062,7 @@
         <v>59</v>
       </c>
       <c r="Q11" t="n">
-        <v>27020</v>
+        <v>1125.83</v>
       </c>
     </row>
     <row r="12">
@@ -1117,7 +1117,7 @@
         <v>55</v>
       </c>
       <c r="Q12" t="n">
-        <v>26648</v>
+        <v>1110.33</v>
       </c>
     </row>
     <row r="13">
@@ -1172,7 +1172,7 @@
         <v>59</v>
       </c>
       <c r="Q13" t="n">
-        <v>24288</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="14">
@@ -1227,7 +1227,7 @@
         <v>51</v>
       </c>
       <c r="Q14" t="n">
-        <v>17554</v>
+        <v>731.42</v>
       </c>
     </row>
     <row r="15">
@@ -1282,7 +1282,7 @@
         <v>47</v>
       </c>
       <c r="Q15" t="n">
-        <v>14804</v>
+        <v>616.83</v>
       </c>
     </row>
     <row r="16">
@@ -1337,7 +1337,7 @@
         <v>42</v>
       </c>
       <c r="Q16" t="n">
-        <v>12492</v>
+        <v>520.5</v>
       </c>
     </row>
     <row r="17">
@@ -1392,7 +1392,7 @@
         <v>42</v>
       </c>
       <c r="Q17" t="n">
-        <v>12294</v>
+        <v>512.25</v>
       </c>
     </row>
     <row r="18">
@@ -1447,7 +1447,7 @@
         <v>29</v>
       </c>
       <c r="Q18" t="n">
-        <v>10480</v>
+        <v>436.67</v>
       </c>
     </row>
     <row r="19">
@@ -1502,7 +1502,7 @@
         <v>43</v>
       </c>
       <c r="Q19" t="n">
-        <v>10200</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20">
@@ -1557,7 +1557,7 @@
         <v>39</v>
       </c>
       <c r="Q20" t="n">
-        <v>9014</v>
+        <v>375.58</v>
       </c>
     </row>
     <row r="21">
@@ -1612,7 +1612,7 @@
         <v>35</v>
       </c>
       <c r="Q21" t="n">
-        <v>8708</v>
+        <v>362.83</v>
       </c>
     </row>
     <row r="22">
@@ -1667,7 +1667,7 @@
         <v>33</v>
       </c>
       <c r="Q22" t="n">
-        <v>7652</v>
+        <v>318.83</v>
       </c>
     </row>
     <row r="23">
@@ -1722,7 +1722,7 @@
         <v>26</v>
       </c>
       <c r="Q23" t="n">
-        <v>6796</v>
+        <v>283.17</v>
       </c>
     </row>
     <row r="24">
@@ -1777,7 +1777,7 @@
         <v>24</v>
       </c>
       <c r="Q24" t="n">
-        <v>6054</v>
+        <v>252.25</v>
       </c>
     </row>
     <row r="25">
@@ -1832,7 +1832,7 @@
         <v>25</v>
       </c>
       <c r="Q25" t="n">
-        <v>5178</v>
+        <v>215.75</v>
       </c>
     </row>
     <row r="26">
@@ -1887,7 +1887,7 @@
         <v>14</v>
       </c>
       <c r="Q26" t="n">
-        <v>4778</v>
+        <v>199.08</v>
       </c>
     </row>
     <row r="27">
@@ -1942,7 +1942,7 @@
         <v>24</v>
       </c>
       <c r="Q27" t="n">
-        <v>4764</v>
+        <v>198.5</v>
       </c>
     </row>
     <row r="28">
@@ -1997,7 +1997,7 @@
         <v>19</v>
       </c>
       <c r="Q28" t="n">
-        <v>4416</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29">
@@ -2052,7 +2052,7 @@
         <v>27</v>
       </c>
       <c r="Q29" t="n">
-        <v>4080</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30">
@@ -2107,7 +2107,7 @@
         <v>16</v>
       </c>
       <c r="Q30" t="n">
-        <v>3756</v>
+        <v>156.5</v>
       </c>
     </row>
     <row r="31">
@@ -2162,7 +2162,7 @@
         <v>20</v>
       </c>
       <c r="Q31" t="n">
-        <v>3672</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32">
@@ -2217,7 +2217,7 @@
         <v>7</v>
       </c>
       <c r="Q32" t="n">
-        <v>3094</v>
+        <v>128.92</v>
       </c>
     </row>
     <row r="33">
@@ -2272,7 +2272,7 @@
         <v>17</v>
       </c>
       <c r="Q33" t="n">
-        <v>3072</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34">
@@ -2327,7 +2327,7 @@
         <v>20</v>
       </c>
       <c r="Q34" t="n">
-        <v>2748</v>
+        <v>114.5</v>
       </c>
     </row>
     <row r="35">
@@ -2382,7 +2382,7 @@
         <v>12</v>
       </c>
       <c r="Q35" t="n">
-        <v>2586</v>
+        <v>107.75</v>
       </c>
     </row>
     <row r="36">
@@ -2437,7 +2437,7 @@
         <v>16</v>
       </c>
       <c r="Q36" t="n">
-        <v>2508</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="37">
@@ -2492,7 +2492,7 @@
         <v>10</v>
       </c>
       <c r="Q37" t="n">
-        <v>2372</v>
+        <v>98.83</v>
       </c>
     </row>
     <row r="38">
@@ -2547,7 +2547,7 @@
         <v>18</v>
       </c>
       <c r="Q38" t="n">
-        <v>2328</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39">
@@ -2602,7 +2602,7 @@
         <v>13</v>
       </c>
       <c r="Q39" t="n">
-        <v>2316</v>
+        <v>96.5</v>
       </c>
     </row>
     <row r="40">
@@ -2657,7 +2657,7 @@
         <v>10</v>
       </c>
       <c r="Q40" t="n">
-        <v>2250</v>
+        <v>93.75</v>
       </c>
     </row>
     <row r="41">
@@ -2712,7 +2712,7 @@
         <v>13</v>
       </c>
       <c r="Q41" t="n">
-        <v>2004</v>
+        <v>83.5</v>
       </c>
     </row>
     <row r="42">
@@ -2767,7 +2767,7 @@
         <v>11</v>
       </c>
       <c r="Q42" t="n">
-        <v>1872</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43">
@@ -2822,7 +2822,7 @@
         <v>14</v>
       </c>
       <c r="Q43" t="n">
-        <v>1776</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44">
@@ -2877,7 +2877,7 @@
         <v>5</v>
       </c>
       <c r="Q44" t="n">
-        <v>1740</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="45">
@@ -2932,7 +2932,7 @@
         <v>9</v>
       </c>
       <c r="Q45" t="n">
-        <v>1608</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46">
@@ -2987,7 +2987,7 @@
         <v>16</v>
       </c>
       <c r="Q46" t="n">
-        <v>1512</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47">
@@ -3042,7 +3042,7 @@
         <v>16</v>
       </c>
       <c r="Q47" t="n">
-        <v>1464</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48">
@@ -3097,7 +3097,7 @@
         <v>12</v>
       </c>
       <c r="Q48" t="n">
-        <v>1440</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49">
@@ -3152,7 +3152,7 @@
         <v>12</v>
       </c>
       <c r="Q49" t="n">
-        <v>1404</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="50">
@@ -3207,7 +3207,7 @@
         <v>16</v>
       </c>
       <c r="Q50" t="n">
-        <v>1368</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51">
@@ -3262,7 +3262,7 @@
         <v>8</v>
       </c>
       <c r="Q51" t="n">
-        <v>1338</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="52">
@@ -3317,7 +3317,7 @@
         <v>11</v>
       </c>
       <c r="Q52" t="n">
-        <v>1284</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="53">
@@ -3372,7 +3372,7 @@
         <v>12</v>
       </c>
       <c r="Q53" t="n">
-        <v>1116</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="54">
@@ -3427,7 +3427,7 @@
         <v>7</v>
       </c>
       <c r="Q54" t="n">
-        <v>1008</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55">
@@ -3482,7 +3482,7 @@
         <v>9</v>
       </c>
       <c r="Q55" t="n">
-        <v>984</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56">
@@ -3537,7 +3537,7 @@
         <v>12</v>
       </c>
       <c r="Q56" t="n">
-        <v>984</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57">
@@ -3592,7 +3592,7 @@
         <v>9</v>
       </c>
       <c r="Q57" t="n">
-        <v>948</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="58">
@@ -3647,7 +3647,7 @@
         <v>12</v>
       </c>
       <c r="Q58" t="n">
-        <v>936</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59">
@@ -3702,7 +3702,7 @@
         <v>6</v>
       </c>
       <c r="Q59" t="n">
-        <v>912</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60">
@@ -3757,7 +3757,7 @@
         <v>6</v>
       </c>
       <c r="Q60" t="n">
-        <v>900</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="61">
@@ -3812,7 +3812,7 @@
         <v>8</v>
       </c>
       <c r="Q61" t="n">
-        <v>900</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="62">
@@ -3867,7 +3867,7 @@
         <v>5</v>
       </c>
       <c r="Q62" t="n">
-        <v>834</v>
+        <v>34.75</v>
       </c>
     </row>
     <row r="63">
@@ -3922,7 +3922,7 @@
         <v>9</v>
       </c>
       <c r="Q63" t="n">
-        <v>828</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="64">
@@ -3977,7 +3977,7 @@
         <v>4</v>
       </c>
       <c r="Q64" t="n">
-        <v>804</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="65">
@@ -4032,7 +4032,7 @@
         <v>6</v>
       </c>
       <c r="Q65" t="n">
-        <v>768</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66">
@@ -4087,7 +4087,7 @@
         <v>4</v>
       </c>
       <c r="Q66" t="n">
-        <v>732</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="67">
@@ -4142,7 +4142,7 @@
         <v>6</v>
       </c>
       <c r="Q67" t="n">
-        <v>696</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68">
@@ -4197,7 +4197,7 @@
         <v>3</v>
       </c>
       <c r="Q68" t="n">
-        <v>684</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="69">
@@ -4252,7 +4252,7 @@
         <v>9</v>
       </c>
       <c r="Q69" t="n">
-        <v>648</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70">
@@ -4307,7 +4307,7 @@
         <v>5</v>
       </c>
       <c r="Q70" t="n">
-        <v>612</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="71">
@@ -4362,7 +4362,7 @@
         <v>9</v>
       </c>
       <c r="Q71" t="n">
-        <v>600</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72">
@@ -4417,7 +4417,7 @@
         <v>5</v>
       </c>
       <c r="Q72" t="n">
-        <v>576</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73">
@@ -4472,7 +4472,7 @@
         <v>3</v>
       </c>
       <c r="Q73" t="n">
-        <v>576</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74">
@@ -4527,7 +4527,7 @@
         <v>8</v>
       </c>
       <c r="Q74" t="n">
-        <v>576</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75">
@@ -4582,7 +4582,7 @@
         <v>5</v>
       </c>
       <c r="Q75" t="n">
-        <v>564</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="76">
@@ -4637,7 +4637,7 @@
         <v>7</v>
       </c>
       <c r="Q76" t="n">
-        <v>552</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77">
@@ -4692,7 +4692,7 @@
         <v>4</v>
       </c>
       <c r="Q77" t="n">
-        <v>528</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78">
@@ -4747,7 +4747,7 @@
         <v>7</v>
       </c>
       <c r="Q78" t="n">
-        <v>528</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79">
@@ -4802,7 +4802,7 @@
         <v>4</v>
       </c>
       <c r="Q79" t="n">
-        <v>516</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="80">
@@ -4857,7 +4857,7 @@
         <v>4</v>
       </c>
       <c r="Q80" t="n">
-        <v>492</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="81">
@@ -4912,7 +4912,7 @@
         <v>3</v>
       </c>
       <c r="Q81" t="n">
-        <v>468</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="82">
@@ -4967,7 +4967,7 @@
         <v>4</v>
       </c>
       <c r="Q82" t="n">
-        <v>468</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="83">
@@ -5022,7 +5022,7 @@
         <v>6</v>
       </c>
       <c r="Q83" t="n">
-        <v>456</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84">
@@ -5077,7 +5077,7 @@
         <v>5</v>
       </c>
       <c r="Q84" t="n">
-        <v>456</v>
+        <v>19</v>
       </c>
     </row>
     <row r="85">
@@ -5132,7 +5132,7 @@
         <v>6</v>
       </c>
       <c r="Q85" t="n">
-        <v>456</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86">
@@ -5187,7 +5187,7 @@
         <v>3</v>
       </c>
       <c r="Q86" t="n">
-        <v>432</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87">
@@ -5242,7 +5242,7 @@
         <v>1</v>
       </c>
       <c r="Q87" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="88">
@@ -5297,7 +5297,7 @@
         <v>4</v>
       </c>
       <c r="Q88" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="89">
@@ -5352,7 +5352,7 @@
         <v>2</v>
       </c>
       <c r="Q89" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="90">
@@ -5407,7 +5407,7 @@
         <v>2</v>
       </c>
       <c r="Q90" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="91">
@@ -5462,7 +5462,7 @@
         <v>2</v>
       </c>
       <c r="Q91" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="92">
@@ -5517,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="Q92" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="93">
@@ -5572,7 +5572,7 @@
         <v>2</v>
       </c>
       <c r="Q93" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="94">
@@ -5627,7 +5627,7 @@
         <v>1</v>
       </c>
       <c r="Q94" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="95">
@@ -5682,7 +5682,7 @@
         <v>2</v>
       </c>
       <c r="Q95" t="n">
-        <v>420</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="96">
@@ -5737,7 +5737,7 @@
         <v>3</v>
       </c>
       <c r="Q96" t="n">
-        <v>396</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="97">
@@ -5792,7 +5792,7 @@
         <v>7</v>
       </c>
       <c r="Q97" t="n">
-        <v>384</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98">
@@ -5847,7 +5847,7 @@
         <v>4</v>
       </c>
       <c r="Q98" t="n">
-        <v>384</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99">
@@ -5902,7 +5902,7 @@
         <v>7</v>
       </c>
       <c r="Q99" t="n">
-        <v>360</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100">
@@ -5957,7 +5957,7 @@
         <v>3</v>
       </c>
       <c r="Q100" t="n">
-        <v>360</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101">
@@ -6012,7 +6012,7 @@
         <v>2</v>
       </c>
       <c r="Q101" t="n">
-        <v>312</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102">
@@ -6067,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="Q102" t="n">
-        <v>300</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="103">
@@ -6122,7 +6122,7 @@
         <v>1</v>
       </c>
       <c r="Q103" t="n">
-        <v>300</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="104">
@@ -6177,7 +6177,7 @@
         <v>3</v>
       </c>
       <c r="Q104" t="n">
-        <v>288</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105">
@@ -6232,7 +6232,7 @@
         <v>2</v>
       </c>
       <c r="Q105" t="n">
-        <v>240</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106">
@@ -6287,7 +6287,7 @@
         <v>2</v>
       </c>
       <c r="Q106" t="n">
-        <v>240</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107">
@@ -6342,7 +6342,7 @@
         <v>5</v>
       </c>
       <c r="Q107" t="n">
-        <v>240</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108">
@@ -6397,7 +6397,7 @@
         <v>2</v>
       </c>
       <c r="Q108" t="n">
-        <v>216</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109">
@@ -6452,7 +6452,7 @@
         <v>4</v>
       </c>
       <c r="Q109" t="n">
-        <v>216</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110">
@@ -6507,7 +6507,7 @@
         <v>1</v>
       </c>
       <c r="Q110" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111">
@@ -6562,7 +6562,7 @@
         <v>1</v>
       </c>
       <c r="Q111" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112">
@@ -6617,7 +6617,7 @@
         <v>3</v>
       </c>
       <c r="Q112" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113">
@@ -6672,7 +6672,7 @@
         <v>1</v>
       </c>
       <c r="Q113" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114">
@@ -6727,7 +6727,7 @@
         <v>3</v>
       </c>
       <c r="Q114" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115">
@@ -6782,7 +6782,7 @@
         <v>3</v>
       </c>
       <c r="Q115" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116">
@@ -6837,7 +6837,7 @@
         <v>1</v>
       </c>
       <c r="Q116" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117">
@@ -6892,7 +6892,7 @@
         <v>1</v>
       </c>
       <c r="Q117" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118">
@@ -6947,7 +6947,7 @@
         <v>1</v>
       </c>
       <c r="Q118" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119">
@@ -7002,7 +7002,7 @@
         <v>1</v>
       </c>
       <c r="Q119" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120">
@@ -7057,7 +7057,7 @@
         <v>2</v>
       </c>
       <c r="Q120" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121">
@@ -7112,7 +7112,7 @@
         <v>1</v>
       </c>
       <c r="Q121" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122">
@@ -7167,7 +7167,7 @@
         <v>1</v>
       </c>
       <c r="Q122" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123">
@@ -7222,7 +7222,7 @@
         <v>3</v>
       </c>
       <c r="Q123" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124">
@@ -7277,7 +7277,7 @@
         <v>3</v>
       </c>
       <c r="Q124" t="n">
-        <v>192</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
@@ -7332,7 +7332,7 @@
         <v>2</v>
       </c>
       <c r="Q125" t="n">
-        <v>168</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126">
@@ -7387,7 +7387,7 @@
         <v>2</v>
       </c>
       <c r="Q126" t="n">
-        <v>144</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127">
@@ -7442,7 +7442,7 @@
         <v>2</v>
       </c>
       <c r="Q127" t="n">
-        <v>144</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128">
@@ -7497,7 +7497,7 @@
         <v>3</v>
       </c>
       <c r="Q128" t="n">
-        <v>144</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129">
@@ -7552,7 +7552,7 @@
         <v>3</v>
       </c>
       <c r="Q129" t="n">
-        <v>144</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130">
@@ -7607,7 +7607,7 @@
         <v>1</v>
       </c>
       <c r="Q130" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131">
@@ -7662,7 +7662,7 @@
         <v>1</v>
       </c>
       <c r="Q131" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
@@ -7717,7 +7717,7 @@
         <v>1</v>
       </c>
       <c r="Q132" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133">
@@ -7772,7 +7772,7 @@
         <v>1</v>
       </c>
       <c r="Q133" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -7827,7 +7827,7 @@
         <v>1</v>
       </c>
       <c r="Q134" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135">
@@ -7882,7 +7882,7 @@
         <v>1</v>
       </c>
       <c r="Q135" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136">
@@ -7937,7 +7937,7 @@
         <v>1</v>
       </c>
       <c r="Q136" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137">
@@ -7992,7 +7992,7 @@
         <v>1</v>
       </c>
       <c r="Q137" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138">
@@ -8047,7 +8047,7 @@
         <v>1</v>
       </c>
       <c r="Q138" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
@@ -8102,7 +8102,7 @@
         <v>1</v>
       </c>
       <c r="Q139" t="n">
-        <v>120</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140">
@@ -8157,7 +8157,7 @@
         <v>1</v>
       </c>
       <c r="Q140" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141">
@@ -8212,7 +8212,7 @@
         <v>1</v>
       </c>
       <c r="Q141" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142">
@@ -8267,7 +8267,7 @@
         <v>2</v>
       </c>
       <c r="Q142" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
@@ -8322,7 +8322,7 @@
         <v>2</v>
       </c>
       <c r="Q143" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144">
@@ -8377,7 +8377,7 @@
         <v>1</v>
       </c>
       <c r="Q144" t="n">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145">
@@ -8432,7 +8432,7 @@
         <v>2</v>
       </c>
       <c r="Q145" t="n">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
@@ -8487,7 +8487,7 @@
         <v>2</v>
       </c>
       <c r="Q146" t="n">
-        <v>72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
@@ -8542,7 +8542,7 @@
         <v>1</v>
       </c>
       <c r="Q147" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
@@ -8597,7 +8597,7 @@
         <v>1</v>
       </c>
       <c r="Q148" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149">
@@ -8652,7 +8652,7 @@
         <v>1</v>
       </c>
       <c r="Q149" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150">
@@ -8707,7 +8707,7 @@
         <v>1</v>
       </c>
       <c r="Q150" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
@@ -8762,7 +8762,7 @@
         <v>2</v>
       </c>
       <c r="Q151" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -8817,7 +8817,7 @@
         <v>2</v>
       </c>
       <c r="Q152" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -8872,7 +8872,7 @@
         <v>1</v>
       </c>
       <c r="Q153" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154">
@@ -8927,7 +8927,7 @@
         <v>2</v>
       </c>
       <c r="Q154" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
@@ -8982,7 +8982,7 @@
         <v>1</v>
       </c>
       <c r="Q155" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -9037,7 +9037,7 @@
         <v>1</v>
       </c>
       <c r="Q156" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157">
@@ -9092,7 +9092,7 @@
         <v>1</v>
       </c>
       <c r="Q157" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -9147,7 +9147,7 @@
         <v>1</v>
       </c>
       <c r="Q158" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -9202,7 +9202,7 @@
         <v>1</v>
       </c>
       <c r="Q159" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -9257,7 +9257,7 @@
         <v>1</v>
       </c>
       <c r="Q160" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -9312,7 +9312,7 @@
         <v>1</v>
       </c>
       <c r="Q161" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -9367,7 +9367,7 @@
         <v>1</v>
       </c>
       <c r="Q162" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -9422,7 +9422,7 @@
         <v>1</v>
       </c>
       <c r="Q163" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>